<commit_message>
Schema changed. Added commissions filter 'Sent on commission'
</commit_message>
<xml_diff>
--- a/DatabaseUpdate/ExcelFiles/CommissionFilters.xlsx
+++ b/DatabaseUpdate/ExcelFiles/CommissionFilters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -77,6 +77,15 @@
   </x:si>
   <x:si>
     <x:t>|awaiting|</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Направлены на комиссию</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|sentOnCommission|</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -427,7 +436,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C7"/>
+  <x:dimension ref="A1:C8"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -510,6 +519,17 @@
         <x:v>20</x:v>
       </x:c>
     </x:row>
+    <x:row r="8" spans="1:3">
+      <x:c r="A8" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>